<commit_message>
Remove -1 to 1 restriction on ecoregion and disturbance modifiers. Recompile. Additional tests for interaction with climate and biomass insects.
git-svn-id: http://Marc-PC/svn/Full@3763 85f15e0e-5137-b144-a863-98bd542365a3
</commit_message>
<xml_diff>
--- a/trunk/base-BDA/branches/base-BDA-v3-climate/tests/v3-climate/examplePDSI.xlsx
+++ b/trunk/base-BDA/branches/base-BDA-v3-climate/tests/v3-climate/examplePDSI.xlsx
@@ -850,7 +850,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -867,7 +869,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3.6665760000000001</v>
+        <v>2.4208609999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.53319819999999996</v>
+        <v>1.518062</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -883,7 +885,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>5.8801050000000004</v>
+        <v>-3.7629480000000002</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -891,7 +893,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2.9426329999999998</v>
+        <v>-3.4316580000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -899,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4.3811770000000001</v>
+        <v>-5.4386450000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -907,7 +909,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.4977259</v>
+        <v>2.2014499999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -915,7 +917,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2.4208609999999999</v>
+        <v>-5.4881450000000003</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -923,7 +925,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1.518062</v>
+        <v>0.33354400000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -931,7 +933,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-3.7629480000000002</v>
+        <v>-0.74709420000000004</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -939,7 +941,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-3.4316580000000001</v>
+        <v>1.6844300000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -947,7 +949,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-5.4386450000000002</v>
+        <v>5.8378560000000004</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -955,7 +957,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2.2014499999999999</v>
+        <v>-1.3282579999999999</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -963,7 +965,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-5.4881450000000003</v>
+        <v>-3.3866779999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -971,7 +973,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.33354400000000001</v>
+        <v>5.9080190000000004</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -979,7 +981,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-0.74709420000000004</v>
+        <v>5.6046649999999998</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -987,7 +989,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1.6844300000000001</v>
+        <v>-5.412928</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -995,7 +997,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>5.8378560000000004</v>
+        <v>5.5299500000000004</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1003,7 +1005,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-1.3282579999999999</v>
+        <v>0.81269829999999998</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1011,7 +1013,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>-3.3866779999999999</v>
+        <v>-2.2581030000000002</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1019,7 +1021,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>5.9080190000000004</v>
+        <v>3.2220810000000002</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1027,7 +1029,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>5.6046649999999998</v>
+        <v>2.959619</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1035,7 +1037,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-5.412928</v>
+        <v>3.8093590000000002</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1043,7 +1045,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>5.5299500000000004</v>
+        <v>5.7111939999999999</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1051,7 +1053,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.81269829999999998</v>
+        <v>4.959803</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1059,7 +1061,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>-2.2581030000000002</v>
+        <v>4.7288500000000004</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1067,7 +1069,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>3.2220810000000002</v>
+        <v>1.27085</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1075,7 +1077,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>2.959619</v>
+        <v>2.8718439999999998</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1083,7 +1085,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>3.8093590000000002</v>
+        <v>-5.7832109999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1091,7 +1093,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>5.7111939999999999</v>
+        <v>-1.6685239999999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1099,7 +1101,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>4.959803</v>
+        <v>1.219692</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1107,7 +1109,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>4.7288500000000004</v>
+        <v>3.58114</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1115,7 +1117,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>1.27085</v>
+        <v>1.1681900000000001</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,7 +1125,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>2.8718439999999998</v>
+        <v>4.4036080000000002</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1131,7 +1133,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>-5.7832109999999999E-2</v>
+        <v>1.610158</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1139,7 +1141,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>-1.6685239999999999</v>
+        <v>5.2049010000000004</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1147,7 +1149,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1.219692</v>
+        <v>-5.9772150000000002</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1155,7 +1157,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>3.58114</v>
+        <v>4.3687040000000001</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1163,7 +1165,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1.1681900000000001</v>
+        <v>-3.031854</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1171,7 +1173,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>4.4036080000000002</v>
+        <v>0.90040929999999997</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1179,7 +1181,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>1.610158</v>
+        <v>-0.42328179999999999</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1187,7 +1189,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>5.2049010000000004</v>
+        <v>4.3751290000000003</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1195,7 +1197,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>-5.9772150000000002</v>
+        <v>0.65308630000000001</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1203,7 +1205,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>4.3687040000000001</v>
+        <v>-5.1344510000000003</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1211,7 +1213,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>-3.031854</v>
+        <v>-4.0427340000000003</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1219,7 +1221,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>0.90040929999999997</v>
+        <v>2.4137400000000002</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1227,7 +1229,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>-0.42328179999999999</v>
+        <v>-2.6501670000000002</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1235,7 +1237,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>4.3751290000000003</v>
+        <v>8.9058289999999998E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1243,7 +1245,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>0.65308630000000001</v>
+        <v>2.4429419999999999</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1251,7 +1253,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>-5.1344510000000003</v>
+        <v>-5.697819</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1259,7 +1261,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>-4.0427340000000003</v>
+        <v>-4.43771</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1267,7 +1269,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>2.4137400000000002</v>
+        <v>4.7623829999999998</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1275,7 +1277,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>-2.6501670000000002</v>
+        <v>-1.5306690000000001</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1283,7 +1285,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>8.9058289999999998E-2</v>
+        <v>2.064473</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1291,7 +1293,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>2.4429419999999999</v>
+        <v>-0.68478090000000003</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1299,7 +1301,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>-5.697819</v>
+        <v>0.30266510000000002</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1307,7 +1309,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>-4.43771</v>
+        <v>-0.70209589999999999</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1315,7 +1317,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>4.7623829999999998</v>
+        <v>-0.3757819</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1323,7 +1325,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>-1.5306690000000001</v>
+        <v>-5.6205530000000001</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1331,7 +1333,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>2.064473</v>
+        <v>5.9809089999999996</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1339,7 +1341,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>-0.68478090000000003</v>
+        <v>-1.78912</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1347,7 +1349,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>0.30266510000000002</v>
+        <v>1.9701310000000001</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1355,7 +1357,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>-0.70209589999999999</v>
+        <v>4.623634</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1363,7 +1365,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>-0.3757819</v>
+        <v>-1.9985759999999999</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1371,7 +1373,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>-5.6205530000000001</v>
+        <v>-1.1030009999999999</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1379,7 +1381,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>5.9809089999999996</v>
+        <v>-2.6847370000000002</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1387,7 +1389,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>-1.78912</v>
+        <v>3.8512559999999998</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -1395,7 +1397,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>1.9701310000000001</v>
+        <v>-4.1185099999999997</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -1403,7 +1405,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>4.623634</v>
+        <v>-3.3073060000000001</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -1411,7 +1413,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>-1.9985759999999999</v>
+        <v>-3.5037150000000001</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -1419,7 +1421,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>-1.1030009999999999</v>
+        <v>3.0021559999999998</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -1427,7 +1429,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>-2.6847370000000002</v>
+        <v>-0.92394620000000005</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1435,7 +1437,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>3.8512559999999998</v>
+        <v>-4.354266</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -1443,7 +1445,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>-4.1185099999999997</v>
+        <v>1.736197</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -1451,7 +1453,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>-3.3073060000000001</v>
+        <v>5.0829769999999996</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -1459,7 +1461,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>-3.5037150000000001</v>
+        <v>-2.7875169999999998</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -1467,7 +1469,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>3.0021559999999998</v>
+        <v>-2.8471039999999999</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -1475,7 +1477,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>-0.92394620000000005</v>
+        <v>-2.9382579999999998</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -1483,7 +1485,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>-4.354266</v>
+        <v>-0.32302249999999999</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -1491,7 +1493,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>1.736197</v>
+        <v>-4.7417790000000002</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,7 +1501,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>5.0829769999999996</v>
+        <v>3.227703</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1507,7 +1509,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>-2.7875169999999998</v>
+        <v>-1.101232</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -1515,7 +1517,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>-2.8471039999999999</v>
+        <v>3.812125</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -1523,7 +1525,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>-2.9382579999999998</v>
+        <v>-5.0173649999999999</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -1531,7 +1533,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>-0.32302249999999999</v>
+        <v>-4.4901070000000001</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -1539,7 +1541,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>-4.7417790000000002</v>
+        <v>-0.6011029</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -1547,7 +1549,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>3.227703</v>
+        <v>-0.49903449999999999</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -1555,7 +1557,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>-1.101232</v>
+        <v>-3.0437280000000002</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -1563,7 +1565,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>3.812125</v>
+        <v>0.94157800000000003</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,7 +1573,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>-5.0173649999999999</v>
+        <v>-3.916274</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -1579,7 +1581,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>-4.4901070000000001</v>
+        <v>2.2190660000000002</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -1587,7 +1589,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>-0.6011029</v>
+        <v>3.3262200000000002</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -1595,7 +1597,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>-0.49903449999999999</v>
+        <v>-5.5306940000000004</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1603,7 +1605,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>-3.0437280000000002</v>
+        <v>-0.7706229</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -1611,7 +1613,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>0.94157800000000003</v>
+        <v>-1.5968880000000001</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -1619,7 +1621,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>-3.916274</v>
+        <v>3.6665760000000001</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1627,7 +1629,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>2.2190660000000002</v>
+        <v>0.53319819999999996</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1635,7 +1637,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>3.3262200000000002</v>
+        <v>5.8801050000000004</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1643,7 +1645,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>-5.5306940000000004</v>
+        <v>2.9426329999999998</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1651,7 +1653,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>-0.7706229</v>
+        <v>4.3811770000000001</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1659,7 +1661,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>-1.5968880000000001</v>
+        <v>0.4977259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>